<commit_message>
Edit model and logic.
</commit_message>
<xml_diff>
--- a/assets/天天爆你屏数据表.xlsx
+++ b/assets/天天爆你屏数据表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="玩家装备" sheetId="2" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="冒险岛BOSS" sheetId="1" r:id="rId4"/>
     <sheet name="伤害公式" sheetId="5" r:id="rId5"/>
     <sheet name="术语" sheetId="6" r:id="rId6"/>
+    <sheet name="SP" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -733,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -782,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1380,7 +1381,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1555,4 +1556,24 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>